<commit_message>
user registration - caso de prueba del nombre (criterios y tamaño)
</commit_message>
<xml_diff>
--- a/scrummetrics/excel/ValidEmailUsrReg.xlsx
+++ b/scrummetrics/excel/ValidEmailUsrReg.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24604"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24606"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\git\ScrumMetrics\scrummetrics\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{98F5C2D0-44F4-4A3E-A987-42CB02B596B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D19F0216-1E69-4EEB-B2DC-FBC512FF0D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{50AA2015-A3D3-40F8-85C7-166167C19443}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="4" xr2:uid="{50AA2015-A3D3-40F8-85C7-166167C19443}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
     <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
+    <sheet name="Hoja5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
   <si>
     <t>Nombre</t>
   </si>
@@ -136,6 +137,21 @@
   </si>
   <si>
     <t>P4ssword</t>
+  </si>
+  <si>
+    <t>validmail011@outlook.com</t>
+  </si>
+  <si>
+    <t>jonreyusr010</t>
+  </si>
+  <si>
+    <t>nicppdihyvpnokiardkvwlguymkabqzzlafpqszjwbexngljpkfqdbwsddnpkwmlpfsybljiiwcoxbljyogbaifwnvseqlvxvngdjwotcwdgwssxsvngclquzloafjzsrtufcgjjdsngvrknmvnrrvcuwpfoiyfugxkmwrukutqjmajievheoeezmabzlqojexkyyrnadbzkxqsqqltivskigfgiigthbktpcetllhjjqmhxlhxrcuageakznxpbzz</t>
+  </si>
+  <si>
+    <t>validmail012@outlook.com</t>
+  </si>
+  <si>
+    <t>jonescusr011</t>
   </si>
 </sst>
 </file>
@@ -517,7 +533,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D4"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -604,7 +620,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="A1:D3"/>
+      <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -721,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80A253A2-70F3-431A-8223-0886E01E58BB}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -791,4 +807,62 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73F17C42-DFA9-490C-A24D-01992C3DE98A}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{A65EA0AD-E391-4851-A021-B57989409805}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{B452265E-E515-45EC-BCE8-0EE76EEE9E3D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Project creation - caso de prueba de fecha de inicio
</commit_message>
<xml_diff>
--- a/scrummetrics/excel/ValidEmailUsrReg.xlsx
+++ b/scrummetrics/excel/ValidEmailUsrReg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\git\ScrumMetrics\scrummetrics\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD779981-6A31-4569-964C-0D02743D402C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D312E800-88CC-437B-BD81-221941BB776C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="9" xr2:uid="{50AA2015-A3D3-40F8-85C7-166167C19443}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="10" activeTab="11" xr2:uid="{50AA2015-A3D3-40F8-85C7-166167C19443}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,8 @@
     <sheet name="Hoja8" sheetId="8" r:id="rId8"/>
     <sheet name="Hoja9" sheetId="9" r:id="rId9"/>
     <sheet name="Hoja10" sheetId="10" r:id="rId10"/>
+    <sheet name="Hoja11" sheetId="11" r:id="rId11"/>
+    <sheet name="Hoja12" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="52">
   <si>
     <t>Nombre</t>
   </si>
@@ -178,6 +180,27 @@
   </si>
   <si>
     <t>pepeusername</t>
+  </si>
+  <si>
+    <t>nombre proyecto</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Fecha de inicio</t>
+  </si>
+  <si>
+    <t>Date Test 1</t>
+  </si>
+  <si>
+    <t>project created in order to test the start date</t>
+  </si>
+  <si>
+    <t>Date Test12</t>
+  </si>
+  <si>
+    <t>13 October 2021</t>
   </si>
 </sst>
 </file>
@@ -645,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88935605-37C9-4D20-8C47-C069BB77CC12}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -691,6 +714,116 @@
       </c>
       <c r="D3" t="s">
         <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD2135E2-FA2D-4EED-9F29-75759029CF44}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA6C17A-DBA3-4E6D-A09E-59577DC00D95}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
project creation - caso de prueba descripcion y comienzo de usuarios
</commit_message>
<xml_diff>
--- a/scrummetrics/excel/ValidEmailUsrReg.xlsx
+++ b/scrummetrics/excel/ValidEmailUsrReg.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24606"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\git\ScrumMetrics\scrummetrics\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D312E800-88CC-437B-BD81-221941BB776C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3FD7A7F-76D9-4D6C-8F5D-D63CE9E3DE2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="10" activeTab="11" xr2:uid="{50AA2015-A3D3-40F8-85C7-166167C19443}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="11" activeTab="13" xr2:uid="{50AA2015-A3D3-40F8-85C7-166167C19443}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,8 @@
     <sheet name="Hoja10" sheetId="10" r:id="rId10"/>
     <sheet name="Hoja11" sheetId="11" r:id="rId11"/>
     <sheet name="Hoja12" sheetId="12" r:id="rId12"/>
+    <sheet name="Hoja13" sheetId="13" r:id="rId13"/>
+    <sheet name="Hoja14" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="58">
   <si>
     <t>Nombre</t>
   </si>
@@ -201,6 +203,25 @@
   </si>
   <si>
     <t>13 October 2021</t>
+  </si>
+  <si>
+    <t>description test 1</t>
+  </si>
+  <si>
+    <t>Project created in order to test the description</t>
+  </si>
+  <si>
+    <t>desctest1</t>
+  </si>
+  <si>
+    <t>Length is 12</t>
+  </si>
+  <si>
+    <t>desctest2</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Aenean ac quam consequat, faucibus libero sed, tincidunt justo. Vivamus maximus felis at iaculis pulvinar. Mauris eleifend augue eros, sed fermentum erat lacinia non. Proin vitae tortor imperdiet lorem eleifend interdum. Vestibulum ante ipsum primis in faucibus orci luctus et ultrices posuere cubilia curae; Praesent tempor, dui non euismod dictum, velit mi commodo turpis, eu hendrerit erat justo nec eros. Curabitur congue elit lectus, et ullamcorper sapien cursus quis. Sed et erat consequat, suscipit odio et, facilisis augue. Nam sed efficitur libero. Interdum et malesuada fames ac ante ipsum primis in faucibus. Curabitur placerat a velit ut viverra.
+Cras ornare, lorem non pharetra lacinia, purus diam sollicitudin elit, quis congue tortor dolor id mauris. Donec eget diam fringilla, mattis libero ut, suscipit erat. Nulla quis tortor feugiat, posuere eros at, dapibus dui. Donec finibus euismod dui in bibendum. Suspendisse vitae sapien at erat vestibulum tristique. Quisque accumsan velit at hendrerit pulvinar. Pellentesque egestas luctus risus, vehicula aliquam orci porttitor sit amet. Vivamus id erat porttitor urna porttitor ultrices. Morbi condimentum porttitor justo, sit amet viverra orci commodo a. Donec sollicitudin ullamcorper dui, euismod congue ligula imperdiet et. Integer non neque eros. Nulla eget elit et dui dictum luctus. Mauris massa est, egestas id ultrices sit amet, ornare non ante. Curabitur vulputate iaculis lectus, nec tincidunt lacus iaculis ut. Vivamus metus est, fermentum eget nulla et, elementum fermentum risus.</t>
   </si>
 </sst>
 </file>
@@ -259,11 +280,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -788,7 +812,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA6C17A-DBA3-4E6D-A09E-59577DC00D95}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -823,6 +849,135 @@
         <v>49</v>
       </c>
       <c r="E2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90563B80-C421-4060-A708-8C1637776529}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A1:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{206EB9FE-7D8A-4434-A153-D01920C23B4E}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="409.6">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
create project - ultimos casos de prueba
</commit_message>
<xml_diff>
--- a/scrummetrics/excel/ValidEmailUsrReg.xlsx
+++ b/scrummetrics/excel/ValidEmailUsrReg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\git\ScrumMetrics\scrummetrics\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3FD7A7F-76D9-4D6C-8F5D-D63CE9E3DE2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D55BE3F-DEB7-4BE2-9A75-750AFE2A02DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="11" activeTab="13" xr2:uid="{50AA2015-A3D3-40F8-85C7-166167C19443}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="11" activeTab="15" xr2:uid="{50AA2015-A3D3-40F8-85C7-166167C19443}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,8 @@
     <sheet name="Hoja12" sheetId="12" r:id="rId12"/>
     <sheet name="Hoja13" sheetId="13" r:id="rId13"/>
     <sheet name="Hoja14" sheetId="14" r:id="rId14"/>
+    <sheet name="Hoja15" sheetId="15" r:id="rId15"/>
+    <sheet name="Hoja16" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="65">
   <si>
     <t>Nombre</t>
   </si>
@@ -222,6 +224,27 @@
   <si>
     <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Aenean ac quam consequat, faucibus libero sed, tincidunt justo. Vivamus maximus felis at iaculis pulvinar. Mauris eleifend augue eros, sed fermentum erat lacinia non. Proin vitae tortor imperdiet lorem eleifend interdum. Vestibulum ante ipsum primis in faucibus orci luctus et ultrices posuere cubilia curae; Praesent tempor, dui non euismod dictum, velit mi commodo turpis, eu hendrerit erat justo nec eros. Curabitur congue elit lectus, et ullamcorper sapien cursus quis. Sed et erat consequat, suscipit odio et, facilisis augue. Nam sed efficitur libero. Interdum et malesuada fames ac ante ipsum primis in faucibus. Curabitur placerat a velit ut viverra.
 Cras ornare, lorem non pharetra lacinia, purus diam sollicitudin elit, quis congue tortor dolor id mauris. Donec eget diam fringilla, mattis libero ut, suscipit erat. Nulla quis tortor feugiat, posuere eros at, dapibus dui. Donec finibus euismod dui in bibendum. Suspendisse vitae sapien at erat vestibulum tristique. Quisque accumsan velit at hendrerit pulvinar. Pellentesque egestas luctus risus, vehicula aliquam orci porttitor sit amet. Vivamus id erat porttitor urna porttitor ultrices. Morbi condimentum porttitor justo, sit amet viverra orci commodo a. Donec sollicitudin ullamcorper dui, euismod congue ligula imperdiet et. Integer non neque eros. Nulla eget elit et dui dictum luctus. Mauris massa est, egestas id ultrices sit amet, ornare non ante. Curabitur vulputate iaculis lectus, nec tincidunt lacus iaculis ut. Vivamus metus est, fermentum eget nulla et, elementum fermentum risus.</t>
+  </si>
+  <si>
+    <t>Rol</t>
+  </si>
+  <si>
+    <t>member</t>
+  </si>
+  <si>
+    <t>Team Member</t>
+  </si>
+  <si>
+    <t>asdf123</t>
+  </si>
+  <si>
+    <t>qwer123</t>
+  </si>
+  <si>
+    <t>jositom</t>
+  </si>
+  <si>
+    <t>jonam</t>
   </si>
 </sst>
 </file>
@@ -924,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{206EB9FE-7D8A-4434-A153-D01920C23B4E}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -979,6 +1002,174 @@
       </c>
       <c r="E3" t="s">
         <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F86822BB-723D-4A50-A413-8C932D5F47D3}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF2D3E8B-B54E-419F-A6B6-40EDEC9D9C42}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reportes de login, edit profile y user registration
</commit_message>
<xml_diff>
--- a/scrummetrics/excel/ValidEmailUsrReg.xlsx
+++ b/scrummetrics/excel/ValidEmailUsrReg.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\git\ScrumMetrics\scrummetrics\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D55BE3F-DEB7-4BE2-9A75-750AFE2A02DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1925A5C-ED19-4017-92E5-2218EFEFB988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="11" activeTab="15" xr2:uid="{50AA2015-A3D3-40F8-85C7-166167C19443}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="15" activeTab="1" xr2:uid="{50AA2015-A3D3-40F8-85C7-166167C19443}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
     <t>validmail001@outlook.com</t>
   </si>
   <si>
-    <t>jonreyusrname</t>
+    <t>jonreyusr101</t>
   </si>
   <si>
     <t>P4ssword.</t>
@@ -81,7 +81,7 @@
     <t>validmail001@gmail.com</t>
   </si>
   <si>
-    <t>jonescusrname</t>
+    <t>jonescusr102</t>
   </si>
   <si>
     <t>Abisai Reynosa</t>
@@ -90,25 +90,25 @@
     <t>validmail001@yahoo.com</t>
   </si>
   <si>
-    <t>abireyusrname</t>
+    <t>abireyusr103</t>
   </si>
   <si>
     <t>notvalidmail001</t>
   </si>
   <si>
-    <t>jonreyusr001</t>
+    <t>jonreyusr104</t>
   </si>
   <si>
     <t>not an email</t>
   </si>
   <si>
-    <t>jonescusr002</t>
+    <t>jonescusr105</t>
   </si>
   <si>
     <t>alidmail001@outlook.com</t>
   </si>
   <si>
-    <t>jonreyusr003</t>
+    <t>jonreyusr106</t>
   </si>
   <si>
     <t>P4sswd.</t>
@@ -117,7 +117,7 @@
     <t>samplemail@gmail.com</t>
   </si>
   <si>
-    <t>jonescusr003</t>
+    <t>jonescusr107</t>
   </si>
   <si>
     <t>P4sswordtoolong.</t>
@@ -126,7 +126,7 @@
     <t>validmail010@outlook.com</t>
   </si>
   <si>
-    <t>jonreyusrnames</t>
+    <t>jonreyusr108</t>
   </si>
   <si>
     <t>Password.</t>
@@ -135,7 +135,7 @@
     <t>validmail010@gmail.com</t>
   </si>
   <si>
-    <t>jonescusrnames</t>
+    <t>jonescusr109</t>
   </si>
   <si>
     <t>p4ssword.</t>
@@ -144,7 +144,7 @@
     <t>validmail010@yahoo.com</t>
   </si>
   <si>
-    <t>abireyusrnames</t>
+    <t>abireyusr110</t>
   </si>
   <si>
     <t>P4ssword</t>
@@ -153,7 +153,7 @@
     <t>validmail011@outlook.com</t>
   </si>
   <si>
-    <t>jonreyusr010</t>
+    <t>jonreyusr111</t>
   </si>
   <si>
     <t>nicppdihyvpnokiardkvwlguymkabqzzlafpqszjwbexngljpkfqdbwsddnpkwmlpfsybljiiwcoxbljyogbaifwnvseqlvxvngdjwotcwdgwssxsvngclquzloafjzsrtufcgjjdsngvrknmvnrrvcuwpfoiyfugxkmwrukutqjmajievheoeezmabzlqojexkyyrnadbzkxqsqqltivskigfgiigthbktpcetllhjjqmhxlhxrcuageakznxpbzz</t>
@@ -162,7 +162,7 @@
     <t>validmail012@outlook.com</t>
   </si>
   <si>
-    <t>jonescusr011</t>
+    <t>jonescusr112</t>
   </si>
   <si>
     <t>Jonatan Reynosa 123</t>
@@ -171,7 +171,7 @@
     <t>validmail014@outlook.com</t>
   </si>
   <si>
-    <t>jonreyusr012</t>
+    <t>jonreyusr113</t>
   </si>
   <si>
     <t>Jonatan_Escobedo</t>
@@ -180,7 +180,7 @@
     <t>validmail013@outlook.com</t>
   </si>
   <si>
-    <t>jonescusr012</t>
+    <t>jonescusr114</t>
   </si>
   <si>
     <t>pepeusername</t>
@@ -629,7 +629,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="A1:D4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1097,7 +1097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF2D3E8B-B54E-419F-A6B6-40EDEC9D9C42}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -1181,8 +1181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3882ED02-C607-402A-BE59-C2CF36787966}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1239,7 +1239,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1300,7 +1300,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1376,7 +1376,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="A1:D3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1434,7 +1434,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1553,7 +1553,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
alerta no manejada y ultimo reporte creado user registration
</commit_message>
<xml_diff>
--- a/scrummetrics/excel/ValidEmailUsrReg.xlsx
+++ b/scrummetrics/excel/ValidEmailUsrReg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\git\ScrumMetrics\scrummetrics\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1925A5C-ED19-4017-92E5-2218EFEFB988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{389CF58C-9B71-43CC-A48D-8B50365DCBD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="15" activeTab="1" xr2:uid="{50AA2015-A3D3-40F8-85C7-166167C19443}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" xr2:uid="{50AA2015-A3D3-40F8-85C7-166167C19443}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="68">
   <si>
     <t>Nombre</t>
   </si>
@@ -66,124 +66,133 @@
     <t>Jonatan Reynosa</t>
   </si>
   <si>
+    <t>validmail111@outlook.com</t>
+  </si>
+  <si>
+    <t>jonusr201</t>
+  </si>
+  <si>
+    <t>P4ssword.</t>
+  </si>
+  <si>
+    <t>Jonatan Escobedo</t>
+  </si>
+  <si>
+    <t>validmail211@gmail.com</t>
+  </si>
+  <si>
+    <t>jonusr202</t>
+  </si>
+  <si>
+    <t>Abisai Reynosa</t>
+  </si>
+  <si>
+    <t>validmail311@yahoo.com</t>
+  </si>
+  <si>
+    <t>abiusr203</t>
+  </si>
+  <si>
+    <t>notvalidmail001</t>
+  </si>
+  <si>
+    <t>jonreyusr104</t>
+  </si>
+  <si>
+    <t>not an email</t>
+  </si>
+  <si>
+    <t>jonescusr105</t>
+  </si>
+  <si>
+    <t>alidmail001@outlook.com</t>
+  </si>
+  <si>
+    <t>jonreyusr106</t>
+  </si>
+  <si>
+    <t>P4sswd.</t>
+  </si>
+  <si>
+    <t>samplemail@gmail.com</t>
+  </si>
+  <si>
+    <t>jonescusr107</t>
+  </si>
+  <si>
+    <t>P4sswordtoolong.</t>
+  </si>
+  <si>
+    <t>validmail010@outlook.com</t>
+  </si>
+  <si>
+    <t>jonreyusr108</t>
+  </si>
+  <si>
+    <t>Password.</t>
+  </si>
+  <si>
+    <t>validmail010@gmail.com</t>
+  </si>
+  <si>
+    <t>jonescusr109</t>
+  </si>
+  <si>
+    <t>p4ssword.</t>
+  </si>
+  <si>
+    <t>validmail010@yahoo.com</t>
+  </si>
+  <si>
+    <t>abireyusr110</t>
+  </si>
+  <si>
+    <t>P4ssword</t>
+  </si>
+  <si>
+    <t>validmail011@outlook.com</t>
+  </si>
+  <si>
+    <t>jonreyusr111</t>
+  </si>
+  <si>
+    <t>nicppdihyvpnokiardkvwlguymkabqzzlafpqszjwbexngljpkfqdbwsddnpkwmlpfsybljiiwcoxbljyogbaifwnvseqlvxvngdjwotcwdgwssxsvngclquzloafjzsrtufcgjjdsngvrknmvnrrvcuwpfoiyfugxkmwrukutqjmajievheoeezmabzlqojexkyyrnadbzkxqsqqltivskigfgiigthbktpcetllhjjqmhxlhxrcuageakznxpbzz</t>
+  </si>
+  <si>
+    <t>validmail012@outlook.com</t>
+  </si>
+  <si>
+    <t>jonescusr112</t>
+  </si>
+  <si>
+    <t>Jonatan Reynosa 123</t>
+  </si>
+  <si>
+    <t>validmail014@outlook.com</t>
+  </si>
+  <si>
+    <t>jonreyusr113</t>
+  </si>
+  <si>
+    <t>Jonatan_Escobedo</t>
+  </si>
+  <si>
+    <t>validmail013@outlook.com</t>
+  </si>
+  <si>
+    <t>jonescusr114</t>
+  </si>
+  <si>
+    <t>pepeusername</t>
+  </si>
+  <si>
     <t>validmail001@outlook.com</t>
   </si>
   <si>
-    <t>jonreyusr101</t>
-  </si>
-  <si>
-    <t>P4ssword.</t>
-  </si>
-  <si>
-    <t>Jonatan Escobedo</t>
-  </si>
-  <si>
     <t>validmail001@gmail.com</t>
   </si>
   <si>
-    <t>jonescusr102</t>
-  </si>
-  <si>
-    <t>Abisai Reynosa</t>
-  </si>
-  <si>
     <t>validmail001@yahoo.com</t>
-  </si>
-  <si>
-    <t>abireyusr103</t>
-  </si>
-  <si>
-    <t>notvalidmail001</t>
-  </si>
-  <si>
-    <t>jonreyusr104</t>
-  </si>
-  <si>
-    <t>not an email</t>
-  </si>
-  <si>
-    <t>jonescusr105</t>
-  </si>
-  <si>
-    <t>alidmail001@outlook.com</t>
-  </si>
-  <si>
-    <t>jonreyusr106</t>
-  </si>
-  <si>
-    <t>P4sswd.</t>
-  </si>
-  <si>
-    <t>samplemail@gmail.com</t>
-  </si>
-  <si>
-    <t>jonescusr107</t>
-  </si>
-  <si>
-    <t>P4sswordtoolong.</t>
-  </si>
-  <si>
-    <t>validmail010@outlook.com</t>
-  </si>
-  <si>
-    <t>jonreyusr108</t>
-  </si>
-  <si>
-    <t>Password.</t>
-  </si>
-  <si>
-    <t>validmail010@gmail.com</t>
-  </si>
-  <si>
-    <t>jonescusr109</t>
-  </si>
-  <si>
-    <t>p4ssword.</t>
-  </si>
-  <si>
-    <t>validmail010@yahoo.com</t>
-  </si>
-  <si>
-    <t>abireyusr110</t>
-  </si>
-  <si>
-    <t>P4ssword</t>
-  </si>
-  <si>
-    <t>validmail011@outlook.com</t>
-  </si>
-  <si>
-    <t>jonreyusr111</t>
-  </si>
-  <si>
-    <t>nicppdihyvpnokiardkvwlguymkabqzzlafpqszjwbexngljpkfqdbwsddnpkwmlpfsybljiiwcoxbljyogbaifwnvseqlvxvngdjwotcwdgwssxsvngclquzloafjzsrtufcgjjdsngvrknmvnrrvcuwpfoiyfugxkmwrukutqjmajievheoeezmabzlqojexkyyrnadbzkxqsqqltivskigfgiigthbktpcetllhjjqmhxlhxrcuageakznxpbzz</t>
-  </si>
-  <si>
-    <t>validmail012@outlook.com</t>
-  </si>
-  <si>
-    <t>jonescusr112</t>
-  </si>
-  <si>
-    <t>Jonatan Reynosa 123</t>
-  </si>
-  <si>
-    <t>validmail014@outlook.com</t>
-  </si>
-  <si>
-    <t>jonreyusr113</t>
-  </si>
-  <si>
-    <t>Jonatan_Escobedo</t>
-  </si>
-  <si>
-    <t>validmail013@outlook.com</t>
-  </si>
-  <si>
-    <t>jonescusr114</t>
-  </si>
-  <si>
-    <t>pepeusername</t>
   </si>
   <si>
     <t>nombre proyecto</t>
@@ -628,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47D43E62-999A-4405-A75E-282252FA2453}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -786,13 +795,13 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -803,10 +812,10 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -817,13 +826,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -849,13 +858,13 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -866,13 +875,13 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -898,13 +907,13 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -915,10 +924,10 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -929,13 +938,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -961,13 +970,13 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -978,13 +987,13 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" t="s">
         <v>54</v>
-      </c>
-      <c r="D2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="409.6">
@@ -995,13 +1004,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1027,19 +1036,19 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1050,19 +1059,19 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" t="s">
         <v>54</v>
       </c>
-      <c r="D2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" t="s">
-        <v>51</v>
-      </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1073,19 +1082,19 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
         <v>54</v>
       </c>
-      <c r="D3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" t="s">
-        <v>51</v>
-      </c>
       <c r="F3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1111,19 +1120,19 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1134,19 +1143,19 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" t="s">
         <v>54</v>
       </c>
-      <c r="D2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" t="s">
-        <v>51</v>
-      </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1157,19 +1166,19 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
         <v>54</v>
       </c>
-      <c r="D3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" t="s">
-        <v>51</v>
-      </c>
       <c r="F3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1181,7 +1190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3882ED02-C607-402A-BE59-C2CF36787966}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1638,7 +1647,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -1652,7 +1661,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
         <v>44</v>
@@ -1666,7 +1675,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
         <v>44</v>

</xml_diff>